<commit_message>
added csv outputs in models
</commit_message>
<xml_diff>
--- a/output/JRC/annual_COM_gas_space_heating_bcm.xlsx
+++ b/output/JRC/annual_COM_gas_space_heating_bcm.xlsx
@@ -581,37 +581,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4435238787625809</v>
+        <v>0.4435238787625811</v>
       </c>
       <c r="C3" t="n">
-        <v>0.498736883377578</v>
+        <v>0.4987368833775781</v>
       </c>
       <c r="D3" t="n">
-        <v>0.556352677641354</v>
+        <v>0.5563526776413542</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6162767982973208</v>
+        <v>0.6162767982973212</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6783834518578261</v>
+        <v>0.6783834518578264</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7424721388462294</v>
+        <v>0.7424721388462296</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8083824759151286</v>
+        <v>0.8083824759151288</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8759173185373752</v>
+        <v>0.8759173185373754</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9448396870838849</v>
+        <v>0.9448396870838851</v>
       </c>
       <c r="K3" t="n">
         <v>1.015040176092824</v>
       </c>
       <c r="L3" t="n">
-        <v>1.08634026217635</v>
+        <v>1.086340262176351</v>
       </c>
       <c r="M3" t="n">
         <v>1.158559546002424</v>
@@ -623,22 +623,22 @@
         <v>1.30618188080735</v>
       </c>
       <c r="P3" t="n">
-        <v>1.381401270592732</v>
+        <v>1.381401270592733</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.457422686873269</v>
+        <v>1.45742268687327</v>
       </c>
       <c r="R3" t="n">
-        <v>1.533881450030531</v>
+        <v>1.533881450030532</v>
       </c>
       <c r="S3" t="n">
         <v>1.610758202906694</v>
       </c>
       <c r="T3" t="n">
-        <v>1.687960874161024</v>
+        <v>1.687960874161025</v>
       </c>
       <c r="U3" t="n">
-        <v>1.765368826619229</v>
+        <v>1.76536882661923</v>
       </c>
       <c r="V3" t="n">
         <v>1.843006332147989</v>
@@ -721,52 +721,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4004494393114818</v>
+        <v>0.4004494393114817</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4338685457175808</v>
+        <v>0.4338685457175807</v>
       </c>
       <c r="D5" t="n">
-        <v>0.468650202652991</v>
+        <v>0.4686502026529907</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5047828313595546</v>
+        <v>0.5047828313595545</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5421014947039385</v>
+        <v>0.5421014947039383</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5806225061570006</v>
+        <v>0.5806225061570004</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6204981835975514</v>
+        <v>0.6204981835975512</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6615771416780201</v>
+        <v>0.6615771416780198</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7037682858526377</v>
+        <v>0.7037682858526375</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7470152966701957</v>
+        <v>0.7470152966701954</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7911892789508385</v>
+        <v>0.7911892789508382</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8362893792443364</v>
+        <v>0.8362893792443362</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8822243343013185</v>
+        <v>0.8822243343013183</v>
       </c>
       <c r="O5" t="n">
-        <v>0.9289615776303584</v>
+        <v>0.928961577630358</v>
       </c>
       <c r="P5" t="n">
-        <v>0.9763512560477227</v>
+        <v>0.9763512560477224</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.024403829590553</v>
+        <v>1.024403829590552</v>
       </c>
       <c r="R5" t="n">
         <v>1.073060943408603</v>
@@ -781,7 +781,7 @@
         <v>1.222853542377101</v>
       </c>
       <c r="V5" t="n">
-        <v>1.273806709233427</v>
+        <v>1.273806709233426</v>
       </c>
     </row>
     <row r="6">
@@ -861,22 +861,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07718752367817194</v>
+        <v>0.07718752367817197</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0844638442208278</v>
+        <v>0.08446384422082782</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09192986715359415</v>
+        <v>0.09192986715359419</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0996285032557218</v>
+        <v>0.09962850325572183</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1075624797684794</v>
+        <v>0.1075624797684795</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1157040069907033</v>
+        <v>0.1157040069907034</v>
       </c>
       <c r="H7" t="n">
         <v>0.1240210160109278</v>
@@ -888,16 +888,16 @@
         <v>0.141135057356688</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1498836780967705</v>
+        <v>0.1498836780967706</v>
       </c>
       <c r="L7" t="n">
         <v>0.1587458818039456</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1676885630755617</v>
+        <v>0.1676885630755618</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1766820517148206</v>
+        <v>0.1766820517148207</v>
       </c>
       <c r="O7" t="n">
         <v>0.1857179780645846</v>
@@ -906,22 +906,22 @@
         <v>0.1947978071893965</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2039112372052914</v>
+        <v>0.2039112372052915</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2130487841315319</v>
+        <v>0.213048784131532</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2221985047947869</v>
+        <v>0.222198504794787</v>
       </c>
       <c r="T7" t="n">
-        <v>0.2313501887724492</v>
+        <v>0.2313501887724494</v>
       </c>
       <c r="U7" t="n">
-        <v>0.2405018727501117</v>
+        <v>0.2405018727501118</v>
       </c>
       <c r="V7" t="n">
-        <v>0.2496535567277741</v>
+        <v>0.2496535567277742</v>
       </c>
     </row>
     <row r="8">
@@ -1351,43 +1351,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4804788913367073</v>
+        <v>0.4804788913367075</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5169404750766927</v>
+        <v>0.5169404750766928</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5544910793653576</v>
+        <v>0.5544910793653578</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5929554303432706</v>
+        <v>0.5929554303432708</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6322991586902712</v>
+        <v>0.6322991586902715</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6725003951667119</v>
+        <v>0.6725003951667122</v>
       </c>
       <c r="H14" t="n">
-        <v>0.7134370370613319</v>
+        <v>0.7134370370613323</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7550926550016158</v>
+        <v>0.755092655001616</v>
       </c>
       <c r="J14" t="n">
-        <v>0.79740381713387</v>
+        <v>0.7974038171338702</v>
       </c>
       <c r="K14" t="n">
-        <v>0.840405634895098</v>
+        <v>0.8404056348950982</v>
       </c>
       <c r="L14" t="n">
-        <v>0.8839293691067917</v>
+        <v>0.883929369106792</v>
       </c>
       <c r="M14" t="n">
-        <v>0.9279577874252315</v>
+        <v>0.9279577874252318</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9724128126308913</v>
+        <v>0.9724128126308917</v>
       </c>
       <c r="O14" t="n">
         <v>1.017406586935466</v>
@@ -1396,22 +1396,22 @@
         <v>1.062899079092995</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.108771949982719</v>
+        <v>1.10877194998272</v>
       </c>
       <c r="R14" t="n">
-        <v>1.154980562093149</v>
+        <v>1.15498056209315</v>
       </c>
       <c r="S14" t="n">
-        <v>1.201468698985264</v>
+        <v>1.201468698985265</v>
       </c>
       <c r="T14" t="n">
-        <v>1.248276239767838</v>
+        <v>1.248276239767839</v>
       </c>
       <c r="U14" t="n">
         <v>1.295290529594407</v>
       </c>
       <c r="V14" t="n">
-        <v>1.342454017339493</v>
+        <v>1.342454017339494</v>
       </c>
     </row>
     <row r="15">
@@ -2485,28 +2485,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5263412146825761</v>
+        <v>0.5263412146825763</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5861478140722299</v>
+        <v>0.5861478140722302</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6494421850351773</v>
+        <v>0.6494421850351776</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7157351302051331</v>
+        <v>0.7157351302051334</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7845568368793655</v>
+        <v>0.7845568368793658</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8552044118110552</v>
+        <v>0.8552044118110557</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9276910368446684</v>
+        <v>0.9276910368446686</v>
       </c>
       <c r="I3" t="n">
-        <v>1.001269349265422</v>
+        <v>1.001269349265423</v>
       </c>
       <c r="J3" t="n">
         <v>1.075873607529985</v>
@@ -2518,28 +2518,28 @@
         <v>1.227562861609159</v>
       </c>
       <c r="M3" t="n">
-        <v>1.304152975835429</v>
+        <v>1.30415297583543</v>
       </c>
       <c r="N3" t="n">
-        <v>1.381035111133135</v>
+        <v>1.381035111133136</v>
       </c>
       <c r="O3" t="n">
-        <v>1.458220786949233</v>
+        <v>1.458220786949234</v>
       </c>
       <c r="P3" t="n">
         <v>1.535689176261797</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.613397820302816</v>
+        <v>1.613397820302817</v>
       </c>
       <c r="R3" t="n">
-        <v>1.691282266726687</v>
+        <v>1.691282266726688</v>
       </c>
       <c r="S3" t="n">
-        <v>1.769302352011061</v>
+        <v>1.769302352011062</v>
       </c>
       <c r="T3" t="n">
-        <v>1.847439844214069</v>
+        <v>1.84743984421407</v>
       </c>
       <c r="U3" t="n">
         <v>1.925638766954392</v>
@@ -2625,43 +2625,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4830334127021867</v>
+        <v>0.4830334127021866</v>
       </c>
       <c r="C5" t="n">
         <v>0.518169434309523</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5543926623860509</v>
+        <v>0.5543926623860508</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5917728963632344</v>
+        <v>0.5917728963632342</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6302961956526547</v>
+        <v>0.6302961956526544</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6698916327882909</v>
+        <v>0.6698916327882907</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7105421392744398</v>
+        <v>0.7105421392744395</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7522527164306384</v>
+        <v>0.7522527164306382</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7950059588585204</v>
+        <v>0.7950059588585202</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8386491949971338</v>
+        <v>0.8386491949971335</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8831750043053046</v>
+        <v>0.8831750043053044</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9285437110461059</v>
+        <v>0.9285437110461057</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9747468827776106</v>
+        <v>0.9747468827776103</v>
       </c>
       <c r="O5" t="n">
         <v>1.021603575429831</v>
@@ -2679,10 +2679,10 @@
         <v>1.214370550603418</v>
       </c>
       <c r="T5" t="n">
-        <v>1.263627769300062</v>
+        <v>1.263627769300061</v>
       </c>
       <c r="U5" t="n">
-        <v>1.313282444964604</v>
+        <v>1.313282444964603</v>
       </c>
       <c r="V5" t="n">
         <v>1.363325164660202</v>
@@ -2765,13 +2765,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08110500807851796</v>
+        <v>0.081105008078518</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08911762274439389</v>
+        <v>0.08911762274439392</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09728605522920611</v>
+        <v>0.09728605522920614</v>
       </c>
       <c r="E7" t="n">
         <v>0.1056158818089859</v>
@@ -2780,34 +2780,34 @@
         <v>0.114081229918292</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1226630490688714</v>
+        <v>0.1226630490688715</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1313556315553129</v>
+        <v>0.131355631555313</v>
       </c>
       <c r="I7" t="n">
         <v>0.1401748858341653</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1491039508576596</v>
+        <v>0.1491039508576597</v>
       </c>
       <c r="K7" t="n">
         <v>0.1581120264166271</v>
       </c>
       <c r="L7" t="n">
-        <v>0.167167071389505</v>
+        <v>0.1671670713895051</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1762574262004313</v>
+        <v>0.1762574262004314</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1853735649941866</v>
+        <v>0.1853735649941867</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1945082793137239</v>
+        <v>0.194508279313724</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2036544567945881</v>
+        <v>0.2036544567945882</v>
       </c>
       <c r="Q7" t="n">
         <v>0.2128015954880982</v>
@@ -2819,13 +2819,13 @@
         <v>0.2311045091972832</v>
       </c>
       <c r="T7" t="n">
-        <v>0.2402561931749455</v>
+        <v>0.2402561931749456</v>
       </c>
       <c r="U7" t="n">
-        <v>0.249407877152608</v>
+        <v>0.2494078771526081</v>
       </c>
       <c r="V7" t="n">
-        <v>0.2585595611302703</v>
+        <v>0.2585595611302705</v>
       </c>
     </row>
     <row r="8">
@@ -3255,37 +3255,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5880318793194904</v>
+        <v>0.5880318793194906</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6263672035789692</v>
+        <v>0.6263672035789696</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6655335662983727</v>
+        <v>0.6655335662983729</v>
       </c>
       <c r="E14" t="n">
-        <v>0.7055608716612789</v>
+        <v>0.7055608716612792</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7464786302278666</v>
+        <v>0.7464786302278669</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7881821416321217</v>
+        <v>0.7881821416321221</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8305644574033167</v>
+        <v>0.8305644574033172</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8736066258163258</v>
+        <v>0.8736066258163262</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9172106553613258</v>
+        <v>0.9172106553613262</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9613711222222944</v>
+        <v>0.9613711222222948</v>
       </c>
       <c r="L14" t="n">
-        <v>1.005936809544286</v>
+        <v>1.005936809544287</v>
       </c>
       <c r="M14" t="n">
         <v>1.050883237398111</v>
@@ -3300,7 +3300,7 @@
         <v>1.187692833095823</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.233821878031425</v>
+        <v>1.233821878031426</v>
       </c>
       <c r="R14" t="n">
         <v>1.280198401584491</v>
@@ -3309,10 +3309,10 @@
         <v>1.326801606401742</v>
       </c>
       <c r="T14" t="n">
-        <v>1.373567954188444</v>
+        <v>1.373567954188445</v>
       </c>
       <c r="U14" t="n">
-        <v>1.420559524648125</v>
+        <v>1.420559524648126</v>
       </c>
       <c r="V14" t="n">
         <v>1.467800652827513</v>
@@ -4389,25 +4389,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6402138285320262</v>
+        <v>0.6402138285320265</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7064132311843093</v>
+        <v>0.7064132311843095</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7750547002535011</v>
+        <v>0.7750547002535013</v>
       </c>
       <c r="E3" t="n">
-        <v>0.845500523975426</v>
+        <v>0.8455005239754262</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9174976683042642</v>
+        <v>0.9174976683042645</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9908358603522772</v>
+        <v>0.9908358603522777</v>
       </c>
       <c r="H3" t="n">
-        <v>1.065287070372799</v>
+        <v>1.0652870703728</v>
       </c>
       <c r="I3" t="n">
         <v>1.140629788195556</v>
@@ -4422,34 +4422,34 @@
         <v>1.370657482656765</v>
       </c>
       <c r="M3" t="n">
-        <v>1.448198113391397</v>
+        <v>1.448198113391398</v>
       </c>
       <c r="N3" t="n">
-        <v>1.5260414643876</v>
+        <v>1.526041464387601</v>
       </c>
       <c r="O3" t="n">
-        <v>1.604141805258828</v>
+        <v>1.604141805258829</v>
       </c>
       <c r="P3" t="n">
-        <v>1.682440805467855</v>
+        <v>1.682440805467856</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.760935069171737</v>
+        <v>1.760935069171738</v>
       </c>
       <c r="R3" t="n">
-        <v>1.839558490963632</v>
+        <v>1.839558490963633</v>
       </c>
       <c r="S3" t="n">
-        <v>1.918194668303093</v>
+        <v>1.918194668303094</v>
       </c>
       <c r="T3" t="n">
-        <v>1.996830845642555</v>
+        <v>1.996830845642556</v>
       </c>
       <c r="U3" t="n">
-        <v>2.075467022982016</v>
+        <v>2.075467022982017</v>
       </c>
       <c r="V3" t="n">
-        <v>2.154103200321478</v>
+        <v>2.154103200321479</v>
       </c>
     </row>
     <row r="4">
@@ -4529,55 +4529,55 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5942928422966876</v>
+        <v>0.5942928422966874</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6323038921463215</v>
+        <v>0.6323038921463213</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6712843387388961</v>
+        <v>0.6712843387388959</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7114532177914286</v>
+        <v>0.7114532177914284</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7528255806888625</v>
+        <v>0.7528255806888623</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7952009106981081</v>
+        <v>0.7952009106981078</v>
       </c>
       <c r="H5" t="n">
-        <v>0.838543428766646</v>
+        <v>0.8385434287666457</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8829028168172212</v>
+        <v>0.8829028168172208</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9281798380873629</v>
+        <v>0.9281798380873625</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9742588657766523</v>
+        <v>0.9742588657766522</v>
       </c>
       <c r="L5" t="n">
         <v>1.021153914529358</v>
       </c>
       <c r="M5" t="n">
-        <v>1.068835669704442</v>
+        <v>1.068835669704441</v>
       </c>
       <c r="N5" t="n">
         <v>1.117176742769685</v>
       </c>
       <c r="O5" t="n">
-        <v>1.166106433637038</v>
+        <v>1.166106433637037</v>
       </c>
       <c r="P5" t="n">
-        <v>1.215576832170333</v>
+        <v>1.215576832170332</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.265559575076632</v>
+        <v>1.265559575076631</v>
       </c>
       <c r="R5" t="n">
-        <v>1.316007469207742</v>
+        <v>1.316007469207741</v>
       </c>
       <c r="S5" t="n">
         <v>1.366955346992172</v>
@@ -4589,7 +4589,7 @@
         <v>1.470055691135288</v>
       </c>
       <c r="V5" t="n">
-        <v>1.522038741166794</v>
+        <v>1.522038741166793</v>
       </c>
     </row>
     <row r="6">
@@ -4669,37 +4669,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1048499460819555</v>
+        <v>0.1048499460819556</v>
       </c>
       <c r="C7" t="n">
         <v>0.1132310069140282</v>
       </c>
       <c r="D7" t="n">
-        <v>0.121708597190014</v>
+        <v>0.1217085971900141</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1302936808453269</v>
+        <v>0.130293680845327</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1389802516753155</v>
+        <v>0.1389802516753156</v>
       </c>
       <c r="G7" t="n">
         <v>0.1477610312603266</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1566159827912404</v>
+        <v>0.1566159827912405</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1655270188878837</v>
+        <v>0.1655270188878838</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1744954683726455</v>
+        <v>0.1744954683726456</v>
       </c>
       <c r="K7" t="n">
         <v>0.1835155915065789</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1925753502293044</v>
+        <v>0.1925753502293045</v>
       </c>
       <c r="M7" t="n">
         <v>0.2016720047947292</v>
@@ -4708,28 +4708,28 @@
         <v>0.2107831290844802</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2199095833250038</v>
+        <v>0.2199095833250039</v>
       </c>
       <c r="P7" t="n">
-        <v>0.229052554617572</v>
+        <v>0.2290525546175721</v>
       </c>
       <c r="Q7" t="n">
         <v>0.238202340909649</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2473540248873114</v>
+        <v>0.2473540248873115</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2565057088649737</v>
+        <v>0.2565057088649738</v>
       </c>
       <c r="T7" t="n">
-        <v>0.2656573928426362</v>
+        <v>0.2656573928426363</v>
       </c>
       <c r="U7" t="n">
-        <v>0.2748090768202986</v>
+        <v>0.2748090768202988</v>
       </c>
       <c r="V7" t="n">
-        <v>0.283960760797961</v>
+        <v>0.2839607607979611</v>
       </c>
     </row>
     <row r="8">
@@ -5159,25 +5159,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7065117232126258</v>
+        <v>0.7065117232126261</v>
       </c>
       <c r="C14" t="n">
-        <v>0.74732159022572</v>
+        <v>0.7473215902257202</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7888372329607992</v>
+        <v>0.7888372329607996</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8309980639998007</v>
+        <v>0.8309980639998009</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8736800785405132</v>
+        <v>0.8736800785405134</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9168719548628997</v>
+        <v>0.9168719548629001</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9605710755833857</v>
+        <v>0.9605710755833862</v>
       </c>
       <c r="I14" t="n">
         <v>1.004664273630049</v>
@@ -5195,13 +5195,13 @@
         <v>1.1842556507744</v>
       </c>
       <c r="N14" t="n">
-        <v>1.22974025631131</v>
+        <v>1.229740256311311</v>
       </c>
       <c r="O14" t="n">
-        <v>1.275389999696365</v>
+        <v>1.275389999696366</v>
       </c>
       <c r="P14" t="n">
-        <v>1.321311218562249</v>
+        <v>1.32131121856225</v>
       </c>
       <c r="Q14" t="n">
         <v>1.36743557538075</v>
@@ -5210,10 +5210,10 @@
         <v>1.413750530818659</v>
       </c>
       <c r="S14" t="n">
-        <v>1.460216593316534</v>
+        <v>1.460216593316535</v>
       </c>
       <c r="T14" t="n">
-        <v>1.506886937129334</v>
+        <v>1.506886937129335</v>
       </c>
       <c r="U14" t="n">
         <v>1.553751390907953</v>
@@ -6293,10 +6293,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9111358559237267</v>
+        <v>0.911135855923727</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9743972441194835</v>
+        <v>0.9743972441194839</v>
       </c>
       <c r="D3" t="n">
         <v>1.038905490607616</v>
@@ -6305,13 +6305,13 @@
         <v>1.104705261863225</v>
       </c>
       <c r="F3" t="n">
-        <v>1.171976535428839</v>
+        <v>1.17197653542884</v>
       </c>
       <c r="G3" t="n">
-        <v>1.240799283951524</v>
+        <v>1.240799283951525</v>
       </c>
       <c r="H3" t="n">
-        <v>1.31114109246326</v>
+        <v>1.311141092463261</v>
       </c>
       <c r="I3" t="n">
         <v>1.382653059791956</v>
@@ -6320,10 +6320,10 @@
         <v>1.455240073326364</v>
       </c>
       <c r="K3" t="n">
-        <v>1.528699294818152</v>
+        <v>1.528699294818153</v>
       </c>
       <c r="L3" t="n">
-        <v>1.603052636278925</v>
+        <v>1.603052636278926</v>
       </c>
       <c r="M3" t="n">
         <v>1.678159120462343</v>
@@ -6335,25 +6335,25 @@
         <v>1.829819388052679</v>
       </c>
       <c r="P3" t="n">
-        <v>1.906218955832119</v>
+        <v>1.90621895583212</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.982929265823032</v>
+        <v>1.982929265823034</v>
       </c>
       <c r="R3" t="n">
-        <v>2.059877743924262</v>
+        <v>2.059877743924263</v>
       </c>
       <c r="S3" t="n">
-        <v>2.137059302666552</v>
+        <v>2.137059302666553</v>
       </c>
       <c r="T3" t="n">
-        <v>2.214423238170979</v>
+        <v>2.21442323817098</v>
       </c>
       <c r="U3" t="n">
-        <v>2.291984589384528</v>
+        <v>2.291984589384529</v>
       </c>
       <c r="V3" t="n">
-        <v>2.369751091660649</v>
+        <v>2.369751091660651</v>
       </c>
     </row>
     <row r="4">
@@ -6433,25 +6433,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7350030073629379</v>
+        <v>0.7350030073629377</v>
       </c>
       <c r="C5" t="n">
-        <v>0.774117969334447</v>
+        <v>0.7741179693344469</v>
       </c>
       <c r="D5" t="n">
-        <v>0.81400718079696</v>
+        <v>0.8140071807969598</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8545626160819542</v>
+        <v>0.8545626160819539</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8959957888102306</v>
+        <v>0.8959957888102302</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9382714215947351</v>
+        <v>0.938271421594735</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9814190483894376</v>
+        <v>0.9814190483894372</v>
       </c>
       <c r="I5" t="n">
         <v>1.025402164055872</v>
@@ -6460,7 +6460,7 @@
         <v>1.070106372254546</v>
       </c>
       <c r="K5" t="n">
-        <v>1.115563604024544</v>
+        <v>1.115563604024543</v>
       </c>
       <c r="L5" t="n">
         <v>1.161651980080346</v>
@@ -6472,22 +6472,22 @@
         <v>1.25566185913786</v>
       </c>
       <c r="O5" t="n">
-        <v>1.303536005303371</v>
+        <v>1.30353600530337</v>
       </c>
       <c r="P5" t="n">
         <v>1.351957787453518</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.400885747940882</v>
+        <v>1.400885747940881</v>
       </c>
       <c r="R5" t="n">
         <v>1.450293761600809</v>
       </c>
       <c r="S5" t="n">
-        <v>1.500194567494574</v>
+        <v>1.500194567494573</v>
       </c>
       <c r="T5" t="n">
-        <v>1.550586107330895</v>
+        <v>1.550586107330894</v>
       </c>
       <c r="U5" t="n">
         <v>1.601417582134824</v>
@@ -6576,64 +6576,64 @@
         <v>0.135679404574222</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1440633873202512</v>
+        <v>0.1440633873202513</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1525659696015968</v>
+        <v>0.1525659696015969</v>
       </c>
       <c r="E7" t="n">
         <v>0.1611925176927208</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1699359786081825</v>
+        <v>0.1699359786081826</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1787570565806785</v>
+        <v>0.1787570565806786</v>
       </c>
       <c r="H7" t="n">
         <v>0.1876625177166986</v>
       </c>
       <c r="I7" t="n">
-        <v>0.196635046166133</v>
+        <v>0.1966350461661331</v>
       </c>
       <c r="J7" t="n">
         <v>0.2056551574860689</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2147225559566233</v>
+        <v>0.2147225559566234</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2238171255869605</v>
+        <v>0.2238171255869606</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2329248395469184</v>
+        <v>0.2329248395469185</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2420473342087165</v>
+        <v>0.2420473342087166</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2511746648824505</v>
+        <v>0.2511746648824507</v>
       </c>
       <c r="P7" t="n">
         <v>0.2603096641171243</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2694531636298302</v>
+        <v>0.2694531636298304</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2785990232221075</v>
+        <v>0.2785990232221077</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2877501340528996</v>
+        <v>0.2877501340528997</v>
       </c>
       <c r="T7" t="n">
-        <v>0.296901818030562</v>
+        <v>0.2969018180305621</v>
       </c>
       <c r="U7" t="n">
-        <v>0.3060535020082243</v>
+        <v>0.3060535020082246</v>
       </c>
       <c r="V7" t="n">
-        <v>0.3152051859858868</v>
+        <v>0.3152051859858869</v>
       </c>
     </row>
     <row r="8">
@@ -7063,67 +7063,67 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8156290097724668</v>
+        <v>0.815629009772467</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8589526144000774</v>
+        <v>0.8589526144000776</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9027925947864903</v>
+        <v>0.9027925947864905</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9470300893389446</v>
+        <v>0.9470300893389448</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9916270206188681</v>
+        <v>0.9916270206188688</v>
       </c>
       <c r="G14" t="n">
         <v>1.036647617865927</v>
       </c>
       <c r="H14" t="n">
-        <v>1.082072809555127</v>
+        <v>1.082072809555128</v>
       </c>
       <c r="I14" t="n">
         <v>1.127900430363497</v>
       </c>
       <c r="J14" t="n">
-        <v>1.173948490485137</v>
+        <v>1.173948490485138</v>
       </c>
       <c r="K14" t="n">
         <v>1.220255430847069</v>
       </c>
       <c r="L14" t="n">
-        <v>1.26684428473554</v>
+        <v>1.266844284735541</v>
       </c>
       <c r="M14" t="n">
         <v>1.313726620129928</v>
       </c>
       <c r="N14" t="n">
-        <v>1.360839491769251</v>
+        <v>1.360839491769252</v>
       </c>
       <c r="O14" t="n">
-        <v>1.408045334196706</v>
+        <v>1.408045334196707</v>
       </c>
       <c r="P14" t="n">
         <v>1.455389962913821</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.502836155383499</v>
+        <v>1.5028361553835</v>
       </c>
       <c r="R14" t="n">
-        <v>1.550390123649383</v>
+        <v>1.550390123649384</v>
       </c>
       <c r="S14" t="n">
         <v>1.598040255979359</v>
       </c>
       <c r="T14" t="n">
-        <v>1.645739777074199</v>
+        <v>1.6457397770742</v>
       </c>
       <c r="U14" t="n">
         <v>1.693478626168333</v>
       </c>
       <c r="V14" t="n">
-        <v>1.741256946041837</v>
+        <v>1.741256946041838</v>
       </c>
     </row>
     <row r="15">
@@ -8197,16 +8197,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9650883407483584</v>
+        <v>0.9650883407483588</v>
       </c>
       <c r="C3" t="n">
-        <v>1.032246041012066</v>
+        <v>1.032246041012067</v>
       </c>
       <c r="D3" t="n">
-        <v>1.100534501445869</v>
+        <v>1.10053450144587</v>
       </c>
       <c r="E3" t="n">
-        <v>1.169925454311056</v>
+        <v>1.169925454311057</v>
       </c>
       <c r="F3" t="n">
         <v>1.240282346389688</v>
@@ -8218,46 +8218,46 @@
         <v>1.383444828863135</v>
       </c>
       <c r="I3" t="n">
-        <v>1.456458853214582</v>
+        <v>1.456458853214583</v>
       </c>
       <c r="J3" t="n">
-        <v>1.530307726607955</v>
+        <v>1.530307726607956</v>
       </c>
       <c r="K3" t="n">
-        <v>1.604918706105601</v>
+        <v>1.604918706105602</v>
       </c>
       <c r="L3" t="n">
         <v>1.680159619775047</v>
       </c>
       <c r="M3" t="n">
-        <v>1.75576297590313</v>
+        <v>1.755762975903131</v>
       </c>
       <c r="N3" t="n">
-        <v>1.83171389378934</v>
+        <v>1.831713893789341</v>
       </c>
       <c r="O3" t="n">
-        <v>1.90805330055995</v>
+        <v>1.908053300559951</v>
       </c>
       <c r="P3" t="n">
-        <v>1.984745519484852</v>
+        <v>1.984745519484853</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.061740399136625</v>
+        <v>2.061740399136626</v>
       </c>
       <c r="R3" t="n">
-        <v>2.138991003870553</v>
+        <v>2.138991003870554</v>
       </c>
       <c r="S3" t="n">
         <v>2.216485388123449</v>
       </c>
       <c r="T3" t="n">
-        <v>2.294101499680914</v>
+        <v>2.294101499680915</v>
       </c>
       <c r="U3" t="n">
-        <v>2.371915664564004</v>
+        <v>2.371915664564005</v>
       </c>
       <c r="V3" t="n">
-        <v>2.449830185975126</v>
+        <v>2.449830185975127</v>
       </c>
     </row>
     <row r="4">
@@ -8337,37 +8337,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7837894400536225</v>
+        <v>0.7837894400536223</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8238359989469104</v>
+        <v>0.8238359989469102</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8651316959599906</v>
+        <v>0.8651316959599904</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9075903779845899</v>
+        <v>0.9075903779845894</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9511287938555012</v>
+        <v>0.9511287938555008</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9956855486990359</v>
+        <v>0.9956855486990356</v>
       </c>
       <c r="H5" t="n">
-        <v>1.041196494439755</v>
+        <v>1.041196494439754</v>
       </c>
       <c r="I5" t="n">
         <v>1.087635771067552</v>
       </c>
       <c r="J5" t="n">
-        <v>1.134910855415284</v>
+        <v>1.134910855415283</v>
       </c>
       <c r="K5" t="n">
         <v>1.182889143809797</v>
       </c>
       <c r="L5" t="n">
-        <v>1.231581541485227</v>
+        <v>1.231581541485226</v>
       </c>
       <c r="M5" t="n">
         <v>1.28082127587003</v>
@@ -8388,10 +8388,10 @@
         <v>1.534505540491297</v>
       </c>
       <c r="S5" t="n">
-        <v>1.586469962786127</v>
+        <v>1.586469962786126</v>
       </c>
       <c r="T5" t="n">
-        <v>1.638656577338567</v>
+        <v>1.638656577338566</v>
       </c>
       <c r="U5" t="n">
         <v>1.690984002535134</v>
@@ -8480,64 +8480,64 @@
         <v>0.1498705636743221</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1583199422817814</v>
+        <v>0.1583199422817815</v>
       </c>
       <c r="D7" t="n">
         <v>0.1668953735029099</v>
       </c>
       <c r="E7" t="n">
-        <v>0.175569648928796</v>
+        <v>0.1755696489287961</v>
       </c>
       <c r="F7" t="n">
-        <v>0.184350053904408</v>
+        <v>0.1843500539044081</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1932152301258809</v>
+        <v>0.193215230125881</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2021584783463591</v>
+        <v>0.2021584783463592</v>
       </c>
       <c r="I7" t="n">
-        <v>0.211184096792944</v>
+        <v>0.2111840967929441</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2202669386028353</v>
+        <v>0.2202669386028354</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2293743541982589</v>
+        <v>0.229374354198259</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2384989037621676</v>
+        <v>0.2384989037621677</v>
       </c>
       <c r="M7" t="n">
-        <v>0.247635944215745</v>
+        <v>0.2476359442157451</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2567866917655734</v>
+        <v>0.2567866917655735</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2659383757432358</v>
+        <v>0.2659383757432359</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2750900597208982</v>
+        <v>0.2750900597208983</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2842417436985606</v>
+        <v>0.2842417436985608</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2933934276762231</v>
+        <v>0.2933934276762232</v>
       </c>
       <c r="S7" t="n">
-        <v>0.3025451116538855</v>
+        <v>0.3025451116538856</v>
       </c>
       <c r="T7" t="n">
-        <v>0.3116967956315478</v>
+        <v>0.311696795631548</v>
       </c>
       <c r="U7" t="n">
-        <v>0.3208484796092103</v>
+        <v>0.3208484796092104</v>
       </c>
       <c r="V7" t="n">
-        <v>0.3300001635868726</v>
+        <v>0.3300001635868728</v>
       </c>
     </row>
     <row r="8">
@@ -8967,19 +8967,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8823373082426421</v>
+        <v>0.8823373082426427</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9234026100091418</v>
+        <v>0.9234026100091421</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9652302459972123</v>
+        <v>0.9652302459972129</v>
       </c>
       <c r="E14" t="n">
-        <v>1.007767150660727</v>
+        <v>1.007767150660728</v>
       </c>
       <c r="F14" t="n">
-        <v>1.050897001444458</v>
+        <v>1.050897001444459</v>
       </c>
       <c r="G14" t="n">
         <v>1.094575712073112</v>
@@ -8991,13 +8991,13 @@
         <v>1.183211629126661</v>
       </c>
       <c r="J14" t="n">
-        <v>1.228196538954086</v>
+        <v>1.228196538954087</v>
       </c>
       <c r="K14" t="n">
         <v>1.273520241375758</v>
       </c>
       <c r="L14" t="n">
-        <v>1.319098625355966</v>
+        <v>1.319098625355967</v>
       </c>
       <c r="M14" t="n">
         <v>1.364957387180175</v>
@@ -9006,28 +9006,28 @@
         <v>1.411109706370479</v>
       </c>
       <c r="O14" t="n">
-        <v>1.457568393812551</v>
+        <v>1.457568393812552</v>
       </c>
       <c r="P14" t="n">
-        <v>1.504276794953177</v>
+        <v>1.504276794953178</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.551202922454344</v>
+        <v>1.551202922454345</v>
       </c>
       <c r="R14" t="n">
-        <v>1.598434159374517</v>
+        <v>1.598434159374518</v>
       </c>
       <c r="S14" t="n">
-        <v>1.645842624285895</v>
+        <v>1.645842624285896</v>
       </c>
       <c r="T14" t="n">
-        <v>1.693395600749801</v>
+        <v>1.693395600749802</v>
       </c>
       <c r="U14" t="n">
-        <v>1.741110311990267</v>
+        <v>1.741110311990268</v>
       </c>
       <c r="V14" t="n">
-        <v>1.788910247094094</v>
+        <v>1.788910247094095</v>
       </c>
     </row>
     <row r="15">
@@ -10101,40 +10101,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.858176475016579</v>
+        <v>0.8581764750165793</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9220312914846522</v>
+        <v>0.9220312914846525</v>
       </c>
       <c r="D3" t="n">
-        <v>0.987471239021945</v>
+        <v>0.9874712390219456</v>
       </c>
       <c r="E3" t="n">
         <v>1.054418502787356</v>
       </c>
       <c r="F3" t="n">
-        <v>1.122720171305455</v>
+        <v>1.122720171305456</v>
       </c>
       <c r="G3" t="n">
-        <v>1.192325974447341</v>
+        <v>1.192325974447342</v>
       </c>
       <c r="H3" t="n">
-        <v>1.263302837669143</v>
+        <v>1.263302837669144</v>
       </c>
       <c r="I3" t="n">
-        <v>1.335438222875707</v>
+        <v>1.335438222875708</v>
       </c>
       <c r="J3" t="n">
         <v>1.408465254180287</v>
       </c>
       <c r="K3" t="n">
-        <v>1.482417059445177</v>
+        <v>1.482417059445178</v>
       </c>
       <c r="L3" t="n">
-        <v>1.557083714042876</v>
+        <v>1.557083714042877</v>
       </c>
       <c r="M3" t="n">
-        <v>1.632347091199213</v>
+        <v>1.632347091199214</v>
       </c>
       <c r="N3" t="n">
         <v>1.70809558458783</v>
@@ -10143,25 +10143,25 @@
         <v>1.784403678627184</v>
       </c>
       <c r="P3" t="n">
-        <v>1.861207960392815</v>
+        <v>1.861207960392816</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.93825438288211</v>
+        <v>1.938254382882111</v>
       </c>
       <c r="R3" t="n">
-        <v>2.01548024389154</v>
+        <v>2.015480243891541</v>
       </c>
       <c r="S3" t="n">
         <v>2.092961571718628</v>
       </c>
       <c r="T3" t="n">
-        <v>2.170705863048067</v>
+        <v>2.170705863048068</v>
       </c>
       <c r="U3" t="n">
-        <v>2.248620199800765</v>
+        <v>2.248620199800766</v>
       </c>
       <c r="V3" t="n">
-        <v>2.326621076233339</v>
+        <v>2.32662107623334</v>
       </c>
     </row>
     <row r="4">
@@ -10241,37 +10241,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7837894400536225</v>
+        <v>0.7837894400536223</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8238359989469104</v>
+        <v>0.8238359989469102</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8651316959599906</v>
+        <v>0.8651316959599904</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9075903779845899</v>
+        <v>0.9075903779845894</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9511287938555012</v>
+        <v>0.9511287938555008</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9956855486990359</v>
+        <v>0.9956855486990356</v>
       </c>
       <c r="H5" t="n">
-        <v>1.041196494439755</v>
+        <v>1.041196494439754</v>
       </c>
       <c r="I5" t="n">
         <v>1.087635771067552</v>
       </c>
       <c r="J5" t="n">
-        <v>1.134910855415284</v>
+        <v>1.134910855415283</v>
       </c>
       <c r="K5" t="n">
         <v>1.182889143809797</v>
       </c>
       <c r="L5" t="n">
-        <v>1.231581541485227</v>
+        <v>1.231581541485226</v>
       </c>
       <c r="M5" t="n">
         <v>1.28082127587003</v>
@@ -10292,10 +10292,10 @@
         <v>1.534505540491297</v>
       </c>
       <c r="S5" t="n">
-        <v>1.586469962786127</v>
+        <v>1.586469962786126</v>
       </c>
       <c r="T5" t="n">
-        <v>1.638656577338567</v>
+        <v>1.638656577338566</v>
       </c>
       <c r="U5" t="n">
         <v>1.690984002535134</v>
@@ -10384,64 +10384,64 @@
         <v>0.135679404574222</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1440633873202512</v>
+        <v>0.1440633873202513</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1525659696015968</v>
+        <v>0.1525659696015969</v>
       </c>
       <c r="E7" t="n">
         <v>0.1611925176927208</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1699359786081825</v>
+        <v>0.1699359786081826</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1787570565806785</v>
+        <v>0.1787570565806786</v>
       </c>
       <c r="H7" t="n">
         <v>0.1876625177166986</v>
       </c>
       <c r="I7" t="n">
-        <v>0.196635046166133</v>
+        <v>0.1966350461661331</v>
       </c>
       <c r="J7" t="n">
         <v>0.2056551574860689</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2147225559566233</v>
+        <v>0.2147225559566234</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2238171255869605</v>
+        <v>0.2238171255869606</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2329248395469184</v>
+        <v>0.2329248395469185</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2420473342087165</v>
+        <v>0.2420473342087166</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2511746648824505</v>
+        <v>0.2511746648824507</v>
       </c>
       <c r="P7" t="n">
         <v>0.2603096641171243</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2694531636298302</v>
+        <v>0.2694531636298304</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2785990232221075</v>
+        <v>0.2785990232221077</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2877501340528996</v>
+        <v>0.2877501340528997</v>
       </c>
       <c r="T7" t="n">
-        <v>0.296901818030562</v>
+        <v>0.2969018180305621</v>
       </c>
       <c r="U7" t="n">
-        <v>0.3060535020082243</v>
+        <v>0.3060535020082246</v>
       </c>
       <c r="V7" t="n">
-        <v>0.3152051859858868</v>
+        <v>0.3152051859858869</v>
       </c>
     </row>
     <row r="8">
@@ -10871,19 +10871,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8823373082426421</v>
+        <v>0.8823373082426427</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9234026100091418</v>
+        <v>0.9234026100091421</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9652302459972123</v>
+        <v>0.9652302459972129</v>
       </c>
       <c r="E14" t="n">
-        <v>1.007767150660727</v>
+        <v>1.007767150660728</v>
       </c>
       <c r="F14" t="n">
-        <v>1.050897001444458</v>
+        <v>1.050897001444459</v>
       </c>
       <c r="G14" t="n">
         <v>1.094575712073112</v>
@@ -10895,13 +10895,13 @@
         <v>1.183211629126661</v>
       </c>
       <c r="J14" t="n">
-        <v>1.228196538954086</v>
+        <v>1.228196538954087</v>
       </c>
       <c r="K14" t="n">
         <v>1.273520241375758</v>
       </c>
       <c r="L14" t="n">
-        <v>1.319098625355966</v>
+        <v>1.319098625355967</v>
       </c>
       <c r="M14" t="n">
         <v>1.364957387180175</v>
@@ -10910,28 +10910,28 @@
         <v>1.411109706370479</v>
       </c>
       <c r="O14" t="n">
-        <v>1.457568393812551</v>
+        <v>1.457568393812552</v>
       </c>
       <c r="P14" t="n">
-        <v>1.504276794953177</v>
+        <v>1.504276794953178</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.551202922454344</v>
+        <v>1.551202922454345</v>
       </c>
       <c r="R14" t="n">
-        <v>1.598434159374517</v>
+        <v>1.598434159374518</v>
       </c>
       <c r="S14" t="n">
-        <v>1.645842624285895</v>
+        <v>1.645842624285896</v>
       </c>
       <c r="T14" t="n">
-        <v>1.693395600749801</v>
+        <v>1.693395600749802</v>
       </c>
       <c r="U14" t="n">
-        <v>1.741110311990267</v>
+        <v>1.741110311990268</v>
       </c>
       <c r="V14" t="n">
-        <v>1.788910247094094</v>
+        <v>1.788910247094095</v>
       </c>
     </row>
     <row r="15">
@@ -12005,22 +12005,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6326979466742424</v>
+        <v>0.6326979466742426</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6960209854881478</v>
+        <v>0.6960209854881481</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7617007320230306</v>
+        <v>0.7617007320230309</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8296166237213701</v>
+        <v>0.8296166237213703</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8991035096486704</v>
+        <v>0.8991035096486706</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9698307929000585</v>
+        <v>0.9698307929000589</v>
       </c>
       <c r="H3" t="n">
         <v>1.041703475768383</v>
@@ -12032,7 +12032,7 @@
         <v>1.188655291649564</v>
       </c>
       <c r="K3" t="n">
-        <v>1.263354878863067</v>
+        <v>1.263354878863068</v>
       </c>
       <c r="L3" t="n">
         <v>1.33879068608215</v>
@@ -12041,22 +12041,22 @@
         <v>1.414884623216842</v>
       </c>
       <c r="N3" t="n">
-        <v>1.491369410697033</v>
+        <v>1.491369410697034</v>
       </c>
       <c r="O3" t="n">
         <v>1.568200692810621</v>
       </c>
       <c r="P3" t="n">
-        <v>1.645433642515659</v>
+        <v>1.64543364251566</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.723041392785118</v>
+        <v>1.723041392785119</v>
       </c>
       <c r="R3" t="n">
         <v>1.800949038219549</v>
       </c>
       <c r="S3" t="n">
-        <v>1.879115312087022</v>
+        <v>1.879115312087023</v>
       </c>
       <c r="T3" t="n">
         <v>1.957449129679665</v>
@@ -12065,7 +12065,7 @@
         <v>2.035855350679248</v>
       </c>
       <c r="V3" t="n">
-        <v>2.114357015487599</v>
+        <v>2.1143570154876</v>
       </c>
     </row>
     <row r="4">
@@ -12145,37 +12145,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6232571475801777</v>
+        <v>0.6232571475801776</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6593937598629028</v>
+        <v>0.6593937598629026</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6965340233909569</v>
+        <v>0.6965340233909567</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7347250966148083</v>
+        <v>0.7347250966148082</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7739284634231113</v>
+        <v>0.7739284634231109</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8141163437285036</v>
+        <v>0.8141163437285034</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8551771948278037</v>
+        <v>0.8551771948278035</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8971492276524886</v>
+        <v>0.8971492276524884</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9400761266046505</v>
+        <v>0.9400761266046501</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9838880867044267</v>
+        <v>0.9838880867044265</v>
       </c>
       <c r="L5" t="n">
-        <v>1.028578531681505</v>
+        <v>1.028578531681504</v>
       </c>
       <c r="M5" t="n">
         <v>1.073951614099141</v>
@@ -12184,22 +12184,22 @@
         <v>1.120067173898555</v>
       </c>
       <c r="O5" t="n">
-        <v>1.166831051226781</v>
+        <v>1.16683105122678</v>
       </c>
       <c r="P5" t="n">
-        <v>1.214200545563801</v>
+        <v>1.2142005455638</v>
       </c>
       <c r="Q5" t="n">
         <v>1.262139179830882</v>
       </c>
       <c r="R5" t="n">
-        <v>1.310682374663867</v>
+        <v>1.310682374663866</v>
       </c>
       <c r="S5" t="n">
         <v>1.359845682237431</v>
       </c>
       <c r="T5" t="n">
-        <v>1.409614185132222</v>
+        <v>1.409614185132221</v>
       </c>
       <c r="U5" t="n">
         <v>1.459969038342785</v>
@@ -12294,7 +12294,7 @@
         <v>0.1258660429572304</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1346035678253719</v>
+        <v>0.134603567825372</v>
       </c>
       <c r="F7" t="n">
         <v>0.143439761843815</v>
@@ -12303,7 +12303,7 @@
         <v>0.1523760928653516</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1613909989885727</v>
+        <v>0.1613909989885728</v>
       </c>
       <c r="I7" t="n">
         <v>0.1704642645710171</v>
@@ -12312,40 +12312,40 @@
         <v>0.1795711064464622</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1886987252404985</v>
+        <v>0.1886987252404986</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1978446891319507</v>
+        <v>0.1978446891319508</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2070150484658144</v>
+        <v>0.2070150484658145</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2162041090968166</v>
+        <v>0.2162041090968168</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2253989613951284</v>
+        <v>0.2253989613951285</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2345938136934402</v>
+        <v>0.2345938136934403</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2437886659917519</v>
+        <v>0.243788665991752</v>
       </c>
       <c r="R7" t="n">
-        <v>0.2529835182900637</v>
+        <v>0.2529835182900638</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2621783705883754</v>
+        <v>0.2621783705883756</v>
       </c>
       <c r="T7" t="n">
-        <v>0.2713732228866872</v>
+        <v>0.2713732228866873</v>
       </c>
       <c r="U7" t="n">
-        <v>0.280568075184999</v>
+        <v>0.2805680751849991</v>
       </c>
       <c r="V7" t="n">
-        <v>0.2897629274833107</v>
+        <v>0.2897629274833109</v>
       </c>
     </row>
     <row r="8">
@@ -12775,40 +12775,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6955671409612562</v>
+        <v>0.6955671409612565</v>
       </c>
       <c r="C14" t="n">
-        <v>0.734173746202826</v>
+        <v>0.7341737462028263</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7736632069082952</v>
+        <v>0.7736632069082954</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8139032946350037</v>
+        <v>0.813903294635004</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8548187460224328</v>
+        <v>0.8548187460224332</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8964094521092525</v>
+        <v>0.8964094521092526</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9385612533308221</v>
+        <v>0.9385612533308224</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9813346538732938</v>
+        <v>0.9813346538732942</v>
       </c>
       <c r="J14" t="n">
-        <v>1.024614147626409</v>
+        <v>1.02461414762641</v>
       </c>
       <c r="K14" t="n">
         <v>1.068349607958446</v>
       </c>
       <c r="L14" t="n">
-        <v>1.112592703591854</v>
+        <v>1.112592703591855</v>
       </c>
       <c r="M14" t="n">
-        <v>1.157258358887869</v>
+        <v>1.15725835888787</v>
       </c>
       <c r="N14" t="n">
         <v>1.202348680040285</v>
@@ -12820,22 +12820,22 @@
         <v>1.293386227461661</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.339307801641611</v>
+        <v>1.339307801641612</v>
       </c>
       <c r="R14" t="n">
         <v>1.38546261638843</v>
       </c>
       <c r="S14" t="n">
-        <v>1.431939497356677</v>
+        <v>1.431939497356678</v>
       </c>
       <c r="T14" t="n">
-        <v>1.478672620284438</v>
+        <v>1.478672620284439</v>
       </c>
       <c r="U14" t="n">
-        <v>1.525606004350022</v>
+        <v>1.525606004350023</v>
       </c>
       <c r="V14" t="n">
-        <v>1.5726763236584</v>
+        <v>1.572676323658401</v>
       </c>
     </row>
     <row r="15">

</xml_diff>